<commit_message>
20/04/2025 - PROJECT: 90%
</commit_message>
<xml_diff>
--- a/Logical Design.xlsx
+++ b/Logical Design.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\One_Times\College\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C03DBAC-FBA5-44B4-A091-7671101F5D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9646023E-0C97-452B-B296-068549E4A2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB452E84-88D2-41ED-B9FE-3951C5FD72F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Special" sheetId="1" r:id="rId1"/>
-    <sheet name="Note" sheetId="2" r:id="rId2"/>
+    <sheet name="Add" sheetId="3" r:id="rId2"/>
+    <sheet name="Note" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <r>
       <rPr>
@@ -157,98 +158,9 @@
     <t>PROJECT</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Create Task: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Thiết lập trạng thái mặc định là NOT_STARTED nếu không có</t>
-    </r>
-  </si>
-  <si>
     <t>TASK</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">2. Update Task: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Nếu dueDate được cập nhật thành ngày trong tương lai và status hiện tại là OVER_DUE, cập nhật status thành IN_PROGRESS</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3. Update Task Status:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Nếu trạng thái mới là COMPLETED, cập nhật tất cả subtask thành completed
-- Nếu tất cả tasks đều hoàn thành, cập nhật project thành COMPLETED </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4. Delete Task:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Xóa tất cả subtask</t>
-    </r>
-  </si>
-  <si>
     <t>Thời gian ban đầu</t>
   </si>
   <si>
@@ -277,42 +189,6 @@
   </si>
   <si>
     <t>SUBTASK</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1. Toggle Subtask Status:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Nếu tất cả subtasks đều hoàn thành và task chưa COMPLETED, cập nhật task thành COMPLETED và kiểm tra project
-- Nếu có ít nhất một subtask chưa hoàn thành mà task đang COMPLETED, cập nhật task thành IN_PROGRESS
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nếu tất cả task đã hoàn thành, Cập nhật trạng thái project thành COMPLETED (Nếu lại toggle thành inCompleted thì Task lại thành IN_PROGRESS, vậy Project status có vẻ đang chưa update lại)</t>
-    </r>
   </si>
   <si>
     <t>PROJECT TASK SCHEDULER</t>
@@ -368,6 +244,201 @@
 - Gọi phương thức updateTasksWithCompletedSubtasks để cập nhật task thành COMPLETED nếu tất cả subtask đã hoàn thành
 - Gọi phương thức updateProjectsWithCompletedTasks để cập nhật dự án thành COMPLETED nếu tất cả task đã hoàn thành</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. Update Task: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Nếu dueDate được cập nhật thành ngày trong tương lai và status hiện tại là OVER_DUE, cập nhật status thành IN_PROGRESS
+- Gửi thông báo nếu trạng thái thay đổi</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4. Delete Task:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Xóa tất cả subtask
+- Tạo thông báo về việc xóa công việc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3. Update Task Status:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Gửi thông báo về việc thay đổi trạng thái</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2. Toggle Subtask Status:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Nếu tất cả subtasks đều hoàn thành và task chưa COMPLETED, cập nhật task thành COMPLETED và kiểm tra project
+- Nếu có ít nhất một subtask chưa hoàn thành mà task đang COMPLETED, cập nhật task thành IN_PROGRESS
+- Gửi thông báo đến Project Manager</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7. Khác</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Phần hiển thị thông tin về DueDate (hạn hôm nay, quá hạn bn ngày ...) : chỉ hiển thị quá hạn xxx ngày khi statue không phải completed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Create Task: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Thiết lập trạng thái mặc định là NOT_STARTED nếu không có
+- Gửi thông báo tới project manager, project member về việc tạo công việc mới</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Giới hạn thời lượng tasks k đc quá thời gian kết thúc project</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Create subtask
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Gửi thông báo cho người được giao việc phụ
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Giới hạn thời lượng subtask k đc quá thời gian kết thúc task</t>
+    </r>
+  </si>
+  <si>
+    <t>3. sendDeadlineNotifications
+- Chạy vào phút thứ 30 của mỗi giờ
+-  sendProjectDeadlineNotifications(now, calendar);</t>
   </si>
 </sst>
 </file>
@@ -433,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -447,13 +518,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CACC56E-65EC-46F3-A431-6E5D31AE7C57}">
-  <dimension ref="B1:C20"/>
+  <dimension ref="B1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,57 +893,72 @@
     </row>
     <row r="7" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
-        <v>8</v>
+    <row r="11" spans="2:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>17</v>
+    <row r="21" spans="2:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B23" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -876,18 +968,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC999140-D26F-4E3B-B27E-D592A400BAB6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1D2F6F-27B0-4203-938C-4728F3C6C1BA}">
   <dimension ref="B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
24/04/2025 - Dang code them chuc nang comment
</commit_message>
<xml_diff>
--- a/Logical Design.xlsx
+++ b/Logical Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\One_Times\College\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9646023E-0C97-452B-B296-068549E4A2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E631B298-A2DD-4BD0-9071-4E0AA2EC9979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB452E84-88D2-41ED-B9FE-3951C5FD72F9}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <r>
       <rPr>
@@ -439,13 +439,16 @@
     <t>3. sendDeadlineNotifications
 - Chạy vào phút thứ 30 của mỗi giờ
 -  sendProjectDeadlineNotifications(now, calendar);</t>
+  </si>
+  <si>
+    <t>GỬI THÔNG BÁO CHO AI?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,6 +467,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -525,11 +536,11 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -847,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CACC56E-65EC-46F3-A431-6E5D31AE7C57}">
   <dimension ref="B1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,6 +926,9 @@
       <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="C12" s="9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
@@ -957,7 +971,7 @@
       </c>
     </row>
     <row r="23" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
26/04/2025 - Sua loi linh tinh
</commit_message>
<xml_diff>
--- a/Logical Design.xlsx
+++ b/Logical Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\One_Times\College\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E631B298-A2DD-4BD0-9071-4E0AA2EC9979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1683A7-1C33-4BFB-838C-42A69DF65E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB452E84-88D2-41ED-B9FE-3951C5FD72F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CB452E84-88D2-41ED-B9FE-3951C5FD72F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Special" sheetId="1" r:id="rId1"/>
@@ -38,33 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1. Create Project:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Tạo thông báo cho manager về việc được chỉ định làm quản lý dự án
-- Tạo thông báo cho tất cả thành viên về việc được thêm vào dự án
-- Gửi email thông báo cho manager chứa thông tin chi tiết về dự án và danh sách thành viên</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <r>
       <rPr>
@@ -159,9 +133,6 @@
   </si>
   <si>
     <t>TASK</t>
-  </si>
-  <si>
-    <t>Thời gian ban đầu</t>
   </si>
   <si>
     <r>
@@ -371,45 +342,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">1. Create Task: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Thiết lập trạng thái mặc định là NOT_STARTED nếu không có
-- Gửi thông báo tới project manager, project member về việc tạo công việc mới</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- Giới hạn thời lượng tasks k đc quá thời gian kết thúc project</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">1. Create subtask
 </t>
     </r>
@@ -442,6 +374,120 @@
   </si>
   <si>
     <t>GỬI THÔNG BÁO CHO AI?</t>
+  </si>
+  <si>
+    <t>admin thì thoải mái xóa comment, còn manager và user thì chỉ xóa đc comment của bản thân</t>
+  </si>
+  <si>
+    <t>export excel: còn vấn đề owr sheet task: nên thêm cột assignee</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1. Create Project:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Tạo thông báo cho manager về việc được chỉ định làm quản lý dự án
+- Tạo thông báo cho tất cả thành viên về việc được thêm vào dự án
+- Gửi email thông báo cho manager chứa thông tin chi tiết về dự án và danh sách thành viên
+- Thời lượng Project đang k đc quá 2 năm
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Không đc có quá 20 member (bên ProjectEdit, còn bên ProjectDetail có vẻ chưa check)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Không đc có quá 10 tag (bên ProjectEdit, còn bên ProjectDetail có vẻ chưa check)</t>
+    </r>
+  </si>
+  <si>
+    <t>User thêm ngày sinh</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Create Task: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Thiết lập trạng thái mặc định là NOT_STARTED nếu không có
+- Gửi thông báo tới project manager, project member về việc tạo công việc mới
+- Thời lượng Task đang k đc quá 1 năm</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Giới hạn thời lượng tasks k đc quá thời gian kết thúc project</t>
+    </r>
+  </si>
+  <si>
+    <t>Khi update password cho 1 user, nó chưa bị kích</t>
+  </si>
+  <si>
+    <t>User đang k comment đc</t>
   </si>
 </sst>
 </file>
@@ -858,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CACC56E-65EC-46F3-A431-6E5D31AE7C57}">
   <dimension ref="B1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,106 +919,106 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" ht="72" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="144" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="72" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -985,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC999140-D26F-4E3B-B27E-D592A400BAB6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,17 +1043,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1D2F6F-27B0-4203-938C-4728F3C6C1BA}">
-  <dimension ref="B2"/>
+  <dimension ref="B3:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>7</v>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
26/04/2025 - Trc khi thuc hien gioi han ktg cho Task va SubTask
</commit_message>
<xml_diff>
--- a/Logical Design.xlsx
+++ b/Logical Design.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\One_Times\College\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1683A7-1C33-4BFB-838C-42A69DF65E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CADFD29-3948-4F1A-AB7E-A8C8F9D9396E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CB452E84-88D2-41ED-B9FE-3951C5FD72F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB452E84-88D2-41ED-B9FE-3951C5FD72F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Special" sheetId="1" r:id="rId1"/>
     <sheet name="Add" sheetId="3" r:id="rId2"/>
     <sheet name="Note" sheetId="2" r:id="rId3"/>
+    <sheet name="Ex" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <r>
       <rPr>
@@ -163,58 +164,6 @@
   </si>
   <si>
     <t>PROJECT TASK SCHEDULER</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1. updateOverdueStatus</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Được lên lịch chạy mỗi giờ (vào phút thứ 0 của mỗi giờ)
-- Gọi phương thức updateOverdueProjects để cập nhật các dự án quá hạn
-- Gọi phương thức updateOverdueTasks để cập nhật các task quá hạn</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2. updateCompletedStatus</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Được lên lịch chạy mỗi giờ (vào phút thứ 15 của mỗi giờ)
-- Gọi phương thức updateTasksWithCompletedSubtasks để cập nhật task thành COMPLETED nếu tất cả subtask đã hoàn thành
-- Gọi phương thức updateProjectsWithCompletedTasks để cập nhật dự án thành COMPLETED nếu tất cả task đã hoàn thành</t>
-    </r>
   </si>
   <si>
     <r>
@@ -368,18 +317,160 @@
     </r>
   </si>
   <si>
-    <t>3. sendDeadlineNotifications
-- Chạy vào phút thứ 30 của mỗi giờ
--  sendProjectDeadlineNotifications(now, calendar);</t>
-  </si>
-  <si>
     <t>GỬI THÔNG BÁO CHO AI?</t>
   </si>
   <si>
-    <t>admin thì thoải mái xóa comment, còn manager và user thì chỉ xóa đc comment của bản thân</t>
-  </si>
-  <si>
-    <t>export excel: còn vấn đề owr sheet task: nên thêm cột assignee</t>
+    <r>
+      <t xml:space="preserve">1. Create Task: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Thiết lập trạng thái mặc định là NOT_STARTED nếu không có
+- Gửi thông báo tới project manager, project member về việc tạo công việc mới
+- Thời lượng Task đang k đc quá 1 năm</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Giới hạn thời lượng tasks k đc quá thời gian kết thúc project</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1. Cập nhật trạng thái quá hạn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Được lên lịch chạy mỗi giờ (vào phút thứ 0 của mỗi giờ)
+- Tìm và cập nhật tất cả các Project/ Task đã quá hạn thành status = OVER_DUE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2. Cập nhật trạng thái hoàn thành</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Được lên lịch chạy mỗi giờ (vào phút thứ 0 của mỗi giờ)
+- Cập nhật trạng thái Task thành COMPLETED nếu tất cả các Subtask đều đã hoàn thành
+- Cập nhật trạng thái Project thành COMPLETED nếu tất cả các Task đều đã hoàn thành</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4. Gửi thông báo hạn chót</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Chạy vào phút thứ 0 của mỗi giờ
+-  Gửi thông báo cho Project Manager về các dự án sắp đến hạn (trong vòng 3 ngày) hoặc các dự án đã quá hạn
+- Gửi thông báo cho Project Manager về các Task sắp đến hạn hoặc đã quá hạn
+- Gửi thông báo cho người được giao Subtask khi sắp đến hạn hoặc đã quá hạn</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3. Cập nhật trạng thái IN_PROGRESS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Chạy mỗi giờ (vào phút thứ 0 của mỗi giờ
+- Cập nhật trạng thái Proejct thành IN_PROGRESS nếu có ít nhất 1 Task chưa hoàn thành
+- Cập nhật trạng thái Task thành IN_PROGRESS nếu có ít nhất 1 Subtask chưa hoàn thành</t>
+    </r>
+  </si>
+  <si>
+    <t>Người tạo task và subtask phải là PROJECT MANAGER</t>
+  </si>
+  <si>
+    <t>1. Thêm tokenVersion  vào Users để viết hàm invalid user token để tận dụng cơ chế kiểm tra token hiện có để kích user ra ngoài</t>
+  </si>
+  <si>
+    <t>Hiện tại đang kích user khi disable status bằng hàm check status, sau đó remove user khỏi local storage, cách này k tối ưu</t>
   </si>
   <si>
     <r>
@@ -405,89 +496,8 @@
 - Tạo thông báo cho manager về việc được chỉ định làm quản lý dự án
 - Tạo thông báo cho tất cả thành viên về việc được thêm vào dự án
 - Gửi email thông báo cho manager chứa thông tin chi tiết về dự án và danh sách thành viên
-- Thời lượng Project đang k đc quá 2 năm
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Không đc có quá 20 member (bên ProjectEdit, còn bên ProjectDetail có vẻ chưa check)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- Không đc có quá 10 tag (bên ProjectEdit, còn bên ProjectDetail có vẻ chưa check)</t>
-    </r>
-  </si>
-  <si>
-    <t>User thêm ngày sinh</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Create Task: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Thiết lập trạng thái mặc định là NOT_STARTED nếu không có
-- Gửi thông báo tới project manager, project member về việc tạo công việc mới
-- Thời lượng Task đang k đc quá 1 năm</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- Giới hạn thời lượng tasks k đc quá thời gian kết thúc project</t>
-    </r>
-  </si>
-  <si>
-    <t>Khi update password cho 1 user, nó chưa bị kích</t>
-  </si>
-  <si>
-    <t>User đang k comment đc</t>
+- Thời lượng Project đang k đc quá 2 năm</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -902,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CACC56E-65EC-46F3-A431-6E5D31AE7C57}">
-  <dimension ref="B1:C23"/>
+  <dimension ref="B1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -922,9 +932,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -955,7 +965,7 @@
     </row>
     <row r="8" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
@@ -965,25 +975,25 @@
     </row>
     <row r="11" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
@@ -993,12 +1003,12 @@
     </row>
     <row r="17" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
@@ -1008,17 +1018,22 @@
     </row>
     <row r="21" spans="2:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B23" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1031,7 +1046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC999140-D26F-4E3B-B27E-D592A400BAB6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1043,37 +1058,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1D2F6F-27B0-4203-938C-4728F3C6C1BA}">
-  <dimension ref="B3:B11"/>
+  <dimension ref="B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-    </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4470116-0F26-4A65-970F-AC3E3EE82D95}">
+  <dimension ref="B2:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
26/04/2025 - PROJECT: 90%
</commit_message>
<xml_diff>
--- a/Logical Design.xlsx
+++ b/Logical Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\One_Times\College\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CADFD29-3948-4F1A-AB7E-A8C8F9D9396E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5B4936-5AA2-46CA-982D-8B8E53E887FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB452E84-88D2-41ED-B9FE-3951C5FD72F9}"/>
   </bookViews>
@@ -290,74 +290,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Create subtask
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- Gửi thông báo cho người được giao việc phụ
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- Giới hạn thời lượng subtask k đc quá thời gian kết thúc task</t>
-    </r>
-  </si>
-  <si>
     <t>GỬI THÔNG BÁO CHO AI?</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Create Task: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Thiết lập trạng thái mặc định là NOT_STARTED nếu không có
-- Gửi thông báo tới project manager, project member về việc tạo công việc mới
-- Thời lượng Task đang k đc quá 1 năm</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- Giới hạn thời lượng tasks k đc quá thời gian kết thúc project</t>
-    </r>
   </si>
   <si>
     <r>
@@ -497,6 +430,59 @@
 - Tạo thông báo cho tất cả thành viên về việc được thêm vào dự án
 - Gửi email thông báo cho manager chứa thông tin chi tiết về dự án và danh sách thành viên
 - Thời lượng Project đang k đc quá 2 năm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Create subtask
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Gửi thông báo cho người được giao việc phụ
+- Giới hạn thời lượng Subtask phải thuộc thời lượng Task</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Create Task: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Thiết lập trạng thái mặc định là NOT_STARTED nếu không có
+- Gửi thông báo tới project manager, project member về việc tạo công việc mới
+- Thời lượng Task đang k đc quá 1 năm</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Giới hạn thời lượng Task phải thuộc thời lượng Project</t>
     </r>
   </si>
 </sst>
@@ -504,17 +490,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -531,6 +510,19 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -571,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -582,21 +574,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -914,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CACC56E-65EC-46F3-A431-6E5D31AE7C57}">
   <dimension ref="B1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,7 +929,7 @@
     </row>
     <row r="2" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -974,8 +969,8 @@
       </c>
     </row>
     <row r="11" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
-        <v>16</v>
+      <c r="B11" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -983,7 +978,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1002,8 +997,8 @@
       </c>
     </row>
     <row r="17" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
-        <v>14</v>
+      <c r="B17" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -1018,22 +1013,22 @@
     </row>
     <row r="21" spans="2:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1046,7 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC999140-D26F-4E3B-B27E-D592A400BAB6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1061,14 +1056,14 @@
   <dimension ref="B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1081,19 +1076,19 @@
   <dimension ref="B2:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
27/04/2025 - PROJECT: 90%
</commit_message>
<xml_diff>
--- a/Logical Design.xlsx
+++ b/Logical Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\One_Times\College\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5B4936-5AA2-46CA-982D-8B8E53E887FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58637706-99D2-45BA-9642-966A9FBF2424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB452E84-88D2-41ED-B9FE-3951C5FD72F9}"/>
   </bookViews>
@@ -909,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CACC56E-65EC-46F3-A431-6E5D31AE7C57}">
   <dimension ref="B1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC999140-D26F-4E3B-B27E-D592A400BAB6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1056,7 +1056,7 @@
   <dimension ref="B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
04/05/2025 - Con van de o import Project
</commit_message>
<xml_diff>
--- a/Logical Design.xlsx
+++ b/Logical Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\One_Times\College\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58637706-99D2-45BA-9642-966A9FBF2424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637D1F4F-613A-4435-8185-90D627C15498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB452E84-88D2-41ED-B9FE-3951C5FD72F9}"/>
   </bookViews>
@@ -42,31 +42,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2. Update Project:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Nếu trạng thái hiện tại là OVER_DUE và người dùng cập nhật ngày kết thúc dự kiến (dueDate) thành một ngày trong tương lai, thì tự động cập nhật trạng thái dự án thành IN_PROGRESS
-- Nếu trạng thái thay đổi, tạo thông báo về việc thay đổi trạng thái dự án cho manager và tất cả thành viên</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">3. Add thành viên vào Project:
 </t>
     </r>
@@ -164,31 +139,6 @@
   </si>
   <si>
     <t>PROJECT TASK SCHEDULER</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">2. Update Task: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Nếu dueDate được cập nhật thành ngày trong tương lai và status hiện tại là OVER_DUE, cập nhật status thành IN_PROGRESS
-- Gửi thông báo nếu trạng thái thay đổi</t>
-    </r>
   </si>
   <si>
     <r>
@@ -288,9 +238,6 @@
       <t xml:space="preserve">
 - Phần hiển thị thông tin về DueDate (hạn hôm nay, quá hạn bn ngày ...) : chỉ hiển thị quá hạn xxx ngày khi statue không phải completed</t>
     </r>
-  </si>
-  <si>
-    <t>GỬI THÔNG BÁO CHO AI?</t>
   </si>
   <si>
     <r>
@@ -483,6 +430,60 @@
         <scheme val="minor"/>
       </rPr>
       <t>- Giới hạn thời lượng Task phải thuộc thời lượng Project</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. Update Task: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Nếu dueDate được cập nhật thành ngày trong tương lai và status hiện tại là OVER_DUE, cập nhật status thành IN_PROGRESS
+- Gửi thông báo cho Creator và Manager nếu trạng thái thay đổi</t>
+    </r>
+  </si>
+  <si>
+    <t>Có gửi cho team member không?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2. Update Project:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Nếu trạng thái hiện tại là OVER_DUE và người dùng cập nhật ngày kết thúc dự kiến (dueDate) thành một ngày trong tương lai, thì tự động cập nhật trạng thái dự án thành IN_PROGRESS
+- Nếu trạng thái thay đổi, tạo thông báo về việc thay đổi trạng thái dự án cho manager và tất cả thành viên
+ - Nếu có sự thay đổi về manager của project:  tạo thông báo cho manager cũ, manager mới và team member</t>
     </r>
   </si>
 </sst>
@@ -490,7 +491,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,6 +524,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -584,14 +592,14 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -909,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CACC56E-65EC-46F3-A431-6E5D31AE7C57}">
   <dimension ref="B1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -924,111 +932,112 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
-        <v>13</v>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
-        <v>24</v>
+      <c r="B11" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
-        <v>23</v>
+      <c r="B17" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1063,7 +1072,7 @@
   <sheetData>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1083,12 +1092,12 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
07/05/2025 - Them chuc nang attach files (70%)
</commit_message>
<xml_diff>
--- a/Logical Design.xlsx
+++ b/Logical Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\One_Times\College\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637D1F4F-613A-4435-8185-90D627C15498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B39BBC-C7AE-4E4D-BFD0-23CD35AB7F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB452E84-88D2-41ED-B9FE-3951C5FD72F9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <r>
       <t xml:space="preserve">3. Add thành viên vào Project:
@@ -354,6 +354,76 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">1. Create subtask
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Gửi thông báo cho người được giao việc phụ
+- Giới hạn thời lượng Subtask phải thuộc thời lượng Task</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. Update Task: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Nếu dueDate được cập nhật thành ngày trong tương lai và status hiện tại là OVER_DUE, cập nhật status thành IN_PROGRESS
+- Gửi thông báo cho Creator và Manager nếu trạng thái thay đổi</t>
+    </r>
+  </si>
+  <si>
+    <t>Có gửi cho team member không?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2. Update Project:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Nếu trạng thái hiện tại là OVER_DUE và người dùng cập nhật ngày kết thúc dự kiến (dueDate) thành một ngày trong tương lai, thì tự động cập nhật trạng thái dự án thành IN_PROGRESS
+- Nếu trạng thái thay đổi, tạo thông báo về việc thay đổi trạng thái dự án cho manager và tất cả thành viên
+ - Nếu có sự thay đổi về manager của project:  tạo thông báo cho manager cũ, manager mới và team member</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -376,12 +446,43 @@
 - Tạo thông báo cho manager về việc được chỉ định làm quản lý dự án
 - Tạo thông báo cho tất cả thành viên về việc được thêm vào dự án
 - Gửi email thông báo cho manager chứa thông tin chi tiết về dự án và danh sách thành viên
-- Thời lượng Project đang k đc quá 2 năm</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Create subtask
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Thời lượng Project đang k đc quá 2 năm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Create Task: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Thiết lập trạng thái mặc định là NOT_STARTED nếu không có
+- Gửi thông báo tới project manager, project member về việc tạo công việc mới</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -391,100 +492,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>- Gửi thông báo cho người được giao việc phụ
-- Giới hạn thời lượng Subtask phải thuộc thời lượng Task</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Create Task: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Thiết lập trạng thái mặc định là NOT_STARTED nếu không có
-- Gửi thông báo tới project manager, project member về việc tạo công việc mới
-- Thời lượng Task đang k đc quá 1 năm</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>- Giới hạn thời lượng Task phải thuộc thời lượng Project</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">2. Update Task: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Nếu dueDate được cập nhật thành ngày trong tương lai và status hiện tại là OVER_DUE, cập nhật status thành IN_PROGRESS
-- Gửi thông báo cho Creator và Manager nếu trạng thái thay đổi</t>
-    </r>
-  </si>
-  <si>
-    <t>Có gửi cho team member không?</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2. Update Project:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Nếu trạng thái hiện tại là OVER_DUE và người dùng cập nhật ngày kết thúc dự kiến (dueDate) thành một ngày trong tương lai, thì tự động cập nhật trạng thái dự án thành IN_PROGRESS
-- Nếu trạng thái thay đổi, tạo thông báo về việc thay đổi trạng thái dự án cho manager và tất cả thành viên
- - Nếu có sự thay đổi về manager của project:  tạo thông báo cho manager cũ, manager mới và team member</t>
-    </r>
+    <t>Đang check dup như nào</t>
   </si>
 </sst>
 </file>
@@ -917,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CACC56E-65EC-46F3-A431-6E5D31AE7C57}">
   <dimension ref="B1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -937,12 +949,12 @@
     </row>
     <row r="2" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="10"/>
     </row>
@@ -977,17 +989,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" ht="72" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1005,37 +1017,40 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>